<commit_message>
Writing Code for kon koff data analysis
data extraction complete
currently working on calculating SE values for papers without it
</commit_message>
<xml_diff>
--- a/data/kon_koffs.xlsx
+++ b/data/kon_koffs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/ltukei_uw_edu/Documents/Desktop/GitHub/meta-analysis-for-VEGF-signaling/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lione\Desktop\GitHub\meta-analysis-for-VEGF-signaling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="8_{0383FB71-8A8E-46AC-BA0F-D0C13B61DCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55074E84-ECC0-47BA-A194-1B848517783C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12B8FBF5-D3EB-4F4B-8412-843BC70F4B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15465" yWindow="-1620" windowWidth="15570" windowHeight="9705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16305" yWindow="-1725" windowWidth="16410" windowHeight="14505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
     <t>Method</t>
   </si>
   <si>
-    <t>Kd SE</t>
-  </si>
-  <si>
     <t>Ligand</t>
   </si>
   <si>
@@ -45,16 +42,10 @@
     <t>Kd</t>
   </si>
   <si>
-    <t>kon SE</t>
-  </si>
-  <si>
     <t>kon</t>
   </si>
   <si>
     <t>koff</t>
-  </si>
-  <si>
-    <t>koff SE</t>
   </si>
   <si>
     <t>Recombinant VEGF165 </t>
@@ -161,6 +152,15 @@
   </si>
   <si>
     <t>Mathematical calculation</t>
+  </si>
+  <si>
+    <t>kon SD</t>
+  </si>
+  <si>
+    <t>koff SD</t>
+  </si>
+  <si>
+    <t>Kd SD</t>
   </si>
 </sst>
 </file>
@@ -220,14 +220,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,7 +510,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,51 +526,51 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F2" s="2">
         <v>400000</v>
@@ -594,19 +593,19 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2">
         <v>4000000</v>
@@ -629,19 +628,19 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F4" s="2">
         <v>30000000</v>
@@ -664,19 +663,19 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>23</v>
-      </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F5" s="2">
         <v>1200000</v>
@@ -690,19 +689,19 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F6" s="2">
         <v>2200000</v>
@@ -716,19 +715,19 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F7" s="2">
         <v>1.9E-6</v>
@@ -742,19 +741,19 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F8" s="2">
         <v>2200000</v>
@@ -768,19 +767,19 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
         <v>26</v>
       </c>
-      <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
-      </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F9" s="2">
         <v>3600000</v>
@@ -803,19 +802,19 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F10" s="2">
         <v>5230000</v>
@@ -838,19 +837,19 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
         <v>27</v>
       </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F11" s="2">
         <v>970000</v>
@@ -873,19 +872,19 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F12" s="2">
         <v>500000</v>
@@ -899,19 +898,19 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F13" s="2">
         <v>500000</v>
@@ -925,19 +924,19 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" t="s">
         <v>31</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" t="s">
-        <v>34</v>
       </c>
       <c r="F14" s="2">
         <v>500000</v>
@@ -951,19 +950,19 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" t="s">
         <v>31</v>
-      </c>
-      <c r="B15" t="s">
-        <v>33</v>
-      </c>
-      <c r="C15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" t="s">
-        <v>34</v>
       </c>
       <c r="F15" s="2">
         <v>500000</v>
@@ -977,19 +976,19 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
         <v>33</v>
       </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-      <c r="D16" t="s">
-        <v>36</v>
-      </c>
       <c r="E16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F16" s="2">
         <v>500000</v>
@@ -1003,16 +1002,16 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F17" s="2">
         <v>31000000000000</v>
@@ -1026,17 +1025,17 @@
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
         <v>40</v>
-      </c>
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" t="s">
-        <v>43</v>
       </c>
       <c r="F18" s="2">
         <v>31000000000000</v>
@@ -1047,16 +1046,16 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
         <v>41</v>
-      </c>
-      <c r="B19" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" t="s">
-        <v>44</v>
       </c>
       <c r="F19" s="2">
         <v>300000000000000</v>

</xml_diff>

<commit_message>
add a comma to on of the references to the data
</commit_message>
<xml_diff>
--- a/data/kon_koffs.xlsx
+++ b/data/kon_koffs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lione\Desktop\GitHub\meta-analysis-for-VEGF-signaling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E67F3E-0085-4610-ACD1-D90278C64E11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C8EB54-320E-472D-9847-97211A45FC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="14496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="3156" windowWidth="17280" windowHeight="10548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>VEGF165:VEGR1</t>
   </si>
   <si>
-    <t>von Tiedemann &amp; Bilitewski 2002</t>
-  </si>
-  <si>
     <t>Papadolopulos et al., 2012</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>Kd_SE</t>
+  </si>
+  <si>
+    <t>von Tiedemann &amp; Bilitewski, 2002</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,33 +519,33 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -571,16 +571,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
         <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -606,16 +606,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -641,16 +641,16 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -670,16 +670,16 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -699,16 +699,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -727,16 +727,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -755,16 +755,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -790,16 +790,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -825,16 +825,16 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -860,16 +860,16 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
         <v>19</v>
-      </c>
-      <c r="B12" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
@@ -886,16 +886,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
         <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>
@@ -912,16 +912,16 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
         <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
@@ -938,16 +938,16 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
         <v>19</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>20</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
@@ -964,16 +964,16 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" t="s">
         <v>19</v>
-      </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
-        <v>12</v>
-      </c>
-      <c r="D16" t="s">
-        <v>20</v>
       </c>
       <c r="E16" t="s">
         <v>7</v>
@@ -990,16 +990,16 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
         <v>19</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
@@ -1016,16 +1016,16 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
         <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" t="s">
-        <v>20</v>
       </c>
       <c r="E18" t="s">
         <v>7</v>
@@ -1042,16 +1042,16 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
         <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" t="s">
-        <v>20</v>
       </c>
       <c r="E19" t="s">
         <v>7</v>
@@ -1068,16 +1068,16 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" t="s">
         <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" t="s">
-        <v>20</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Edit the in-house data
</commit_message>
<xml_diff>
--- a/data/kon_koffs.xlsx
+++ b/data/kon_koffs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lione\Desktop\GitHub\meta-analysis-for-VEGF-signaling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD343227-A84E-4863-ADAE-BD69FBD7AE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44056DD4-02BE-4291-B283-53A315E32C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-1845" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="29">
   <si>
     <t xml:space="preserve">Reference </t>
   </si>
@@ -485,21 +485,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +534,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -569,7 +569,7 @@
         <v>2.9999999999999998E-13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -604,7 +604,7 @@
         <v>3.0000000000000001E-12</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -639,7 +639,7 @@
         <v>9.5999999999999995E-13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -668,7 +668,7 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -697,7 +697,7 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -725,7 +725,7 @@
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -753,7 +753,7 @@
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -788,7 +788,7 @@
         <v>4.8999999999999997E-12</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -823,7 +823,7 @@
         <v>5.8000000000000003E-12</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -858,7 +858,7 @@
         <v>4.0000000000000001E-13</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -884,7 +884,7 @@
         <v>7.4300000000000002E-9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -901,196 +901,34 @@
         <v>7</v>
       </c>
       <c r="F13" s="4">
-        <v>581000</v>
+        <v>1010000</v>
       </c>
       <c r="H13" s="2">
-        <v>1.01E-3</v>
+        <v>2.1099999999999999E-3</v>
       </c>
       <c r="J13" s="4">
-        <v>7.4300000000000002E-9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="4">
-        <v>581000</v>
-      </c>
-      <c r="H14" s="2">
-        <v>1.01E-3</v>
-      </c>
-      <c r="J14" s="4">
-        <v>7.4300000000000002E-9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F15" s="4">
-        <v>581000</v>
-      </c>
-      <c r="H15" s="2">
-        <v>1.01E-3</v>
-      </c>
-      <c r="J15" s="4">
-        <v>7.4300000000000002E-9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F16" s="4">
-        <v>1010000</v>
-      </c>
-      <c r="H16" s="2">
-        <v>2.1099999999999999E-3</v>
-      </c>
-      <c r="J16" s="4">
         <v>5.2899999999999997E-9</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F17" s="4">
-        <v>1010000</v>
-      </c>
-      <c r="H17" s="2">
-        <v>2.1099999999999999E-3</v>
-      </c>
-      <c r="J17" s="4">
-        <v>5.2899999999999997E-9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="4">
-        <v>1010000</v>
-      </c>
-      <c r="H18" s="2">
-        <v>2.1099999999999999E-3</v>
-      </c>
-      <c r="J18" s="4">
-        <v>5.2899999999999997E-9</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" t="s">
-        <v>7</v>
-      </c>
-      <c r="F19" s="4">
-        <v>1010000</v>
-      </c>
-      <c r="H19" s="2">
-        <v>2.1099999999999999E-3</v>
-      </c>
-      <c r="J19" s="4">
-        <v>5.2899999999999997E-9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="4">
-        <v>1010000</v>
-      </c>
-      <c r="H20" s="2">
-        <v>2.1099999999999999E-3</v>
-      </c>
-      <c r="J20" s="4">
-        <v>5.2899999999999997E-9</v>
-      </c>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F14" s="4"/>
+      <c r="H14" s="2"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F15" s="4"/>
+      <c r="H15" s="2"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F16" s="4"/>
+      <c r="H16" s="2"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="6:10" x14ac:dyDescent="0.3">
+      <c r="F17" s="4"/>
+      <c r="H17" s="2"/>
+      <c r="J17" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update in house labels in script and the excel sheet
</commit_message>
<xml_diff>
--- a/data/kon_koffs.xlsx
+++ b/data/kon_koffs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lione\Desktop\GitHub\meta-analysis-for-VEGF-signaling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44056DD4-02BE-4291-B283-53A315E32C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F9509B-7603-4FE3-9F2B-882792D2D33B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3456" yWindow="3456" windowWidth="17280" windowHeight="10548" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>VEGF165:VEGR1</t>
   </si>
   <si>
-    <t>Papadolopulos et al., 2012</t>
-  </si>
-  <si>
     <t>VEGF165</t>
   </si>
   <si>
@@ -89,9 +86,6 @@
     <t xml:space="preserve">VEGF165 </t>
   </si>
   <si>
-    <t>Inhouse Data 2023</t>
-  </si>
-  <si>
     <t>NRP1</t>
   </si>
   <si>
@@ -123,6 +117,12 @@
   </si>
   <si>
     <t>​​Mamer et al., 2020</t>
+  </si>
+  <si>
+    <t>In-house data 2023</t>
+  </si>
+  <si>
+    <t>Papadopoulos et al., 2012</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,33 +519,33 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -571,16 +571,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
         <v>7</v>
@@ -606,16 +606,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
@@ -641,16 +641,16 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>7</v>
@@ -670,16 +670,16 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>7</v>
@@ -699,16 +699,16 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>7</v>
@@ -727,16 +727,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
@@ -755,16 +755,16 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
         <v>7</v>
@@ -790,16 +790,16 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>7</v>
@@ -825,16 +825,16 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
@@ -860,16 +860,16 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E12" t="s">
         <v>7</v>
@@ -886,16 +886,16 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
changing Von Tiedemann from SD to SE
</commit_message>
<xml_diff>
--- a/data/kon_koffs.xlsx
+++ b/data/kon_koffs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lione\Desktop\GitHub\meta-analysis-for-VEGF-signaling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8E4016-9A1A-4E2D-9470-066F82BAC71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8549061D-D12E-42CE-A30D-F30CA321669B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -491,7 +491,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,19 +594,22 @@
         <v>4000000</v>
       </c>
       <c r="G3" s="2">
-        <v>1200000</v>
+        <f>1200000/SQRT(10)</f>
+        <v>379473.31922020548</v>
       </c>
       <c r="H3" s="2">
         <v>3.0000000000000001E-5</v>
       </c>
       <c r="I3" s="2">
-        <v>7.9999999999999996E-6</v>
+        <f>0.000008/SQRT(10)</f>
+        <v>2.5298221281347034E-6</v>
       </c>
       <c r="J3" s="2">
         <v>7.5E-12</v>
       </c>
       <c r="K3" s="2">
-        <v>3.0000000000000001E-12</v>
+        <f>0.000000000003/SQRT(10)</f>
+        <v>9.4868329805051386E-13</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding Cunningham et al., 1999 predimer data
</commit_message>
<xml_diff>
--- a/data/kon_koffs.xlsx
+++ b/data/kon_koffs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lione\Desktop\GitHub\meta-analysis-for-VEGF-signaling\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8549061D-D12E-42CE-A30D-F30CA321669B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8327C58A-1709-4426-8850-D818E10EAA45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="14496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="29">
   <si>
     <t xml:space="preserve">Reference </t>
   </si>
@@ -488,23 +488,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="73" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,7 +539,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -574,7 +574,7 @@
         <v>2.9999999999999998E-13</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -612,7 +612,7 @@
         <v>9.4868329805051386E-13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -647,7 +647,7 @@
         <v>9.5999999999999995E-13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -682,7 +682,7 @@
         <v>6.8699999999999996E-12</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -711,7 +711,7 @@
       </c>
       <c r="K6" s="2"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -740,7 +740,7 @@
       </c>
       <c r="K7" s="2"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -768,7 +768,7 @@
       </c>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -796,7 +796,7 @@
       </c>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -831,7 +831,7 @@
         <v>4.8999999999999997E-12</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -866,15 +866,15 @@
         <v>5.8000000000000003E-12</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="D12" t="s">
         <v>19</v>
@@ -883,27 +883,27 @@
         <v>7</v>
       </c>
       <c r="F12" s="2">
-        <v>970000</v>
+        <v>4720000</v>
       </c>
       <c r="G12" s="2">
-        <v>30000</v>
+        <v>1000000</v>
       </c>
       <c r="H12" s="2">
-        <v>9.5000000000000005E-6</v>
+        <v>6.7000000000000002E-5</v>
       </c>
       <c r="I12" s="2">
-        <v>1.9999999999999999E-7</v>
+        <v>1.1E-5</v>
       </c>
       <c r="J12" s="2">
-        <v>9.7999999999999994E-12</v>
+        <v>1.45E-11</v>
       </c>
       <c r="K12" s="2">
-        <v>4.0000000000000001E-13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9.9999999999999998E-13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
@@ -918,28 +918,25 @@
         <v>7</v>
       </c>
       <c r="F13" s="2">
-        <v>669000</v>
+        <v>970000</v>
       </c>
       <c r="G13" s="2">
-        <f>STDEV(F13:F14)/SQRT(2)</f>
-        <v>45500</v>
-      </c>
-      <c r="H13" s="5">
-        <v>5.1500000000000005E-4</v>
+        <v>30000</v>
+      </c>
+      <c r="H13" s="2">
+        <v>9.5000000000000005E-6</v>
       </c>
       <c r="I13" s="2">
-        <f>STDEV(H13:H14)/SQRT(2)</f>
-        <v>1.9750000000000003E-4</v>
-      </c>
-      <c r="J13" s="5">
-        <v>7.7000000000000003E-10</v>
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="J13" s="2">
+        <v>9.7999999999999994E-12</v>
       </c>
       <c r="K13" s="2">
-        <f>STDEV(J13:J14)/SQRT(2)</f>
-        <v>2.5000000000000002E-10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+        <v>4.0000000000000001E-13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -956,54 +953,66 @@
         <v>7</v>
       </c>
       <c r="F14" s="2">
-        <v>578000</v>
+        <v>669000</v>
       </c>
       <c r="G14" s="2">
-        <f>STDEV(F13:F14)/SQRT(2)</f>
+        <f>STDEV(F14:F15)/SQRT(2)</f>
         <v>45500</v>
       </c>
       <c r="H14" s="5">
-        <v>1.2E-4</v>
+        <v>5.1500000000000005E-4</v>
       </c>
       <c r="I14" s="2">
-        <f>STDEV(H13:H14)/SQRT(2)</f>
+        <f>STDEV(H14:H15)/SQRT(2)</f>
         <v>1.9750000000000003E-4</v>
       </c>
       <c r="J14" s="5">
-        <v>2.7E-10</v>
+        <v>7.7000000000000003E-10</v>
       </c>
       <c r="K14" s="2">
-        <f>STDEV(J13:J14)/SQRT(2)</f>
+        <f>STDEV(J14:J15)/SQRT(2)</f>
         <v>2.5000000000000002E-10</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E15" t="s">
         <v>7</v>
       </c>
-      <c r="F15" s="4">
-        <v>581000</v>
-      </c>
-      <c r="H15" s="2">
-        <v>1.01E-3</v>
-      </c>
-      <c r="J15" s="4">
-        <v>7.4300000000000002E-9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F15" s="2">
+        <v>578000</v>
+      </c>
+      <c r="G15" s="2">
+        <f>STDEV(F14:F15)/SQRT(2)</f>
+        <v>45500</v>
+      </c>
+      <c r="H15" s="5">
+        <v>1.2E-4</v>
+      </c>
+      <c r="I15" s="2">
+        <f>STDEV(H14:H15)/SQRT(2)</f>
+        <v>1.9750000000000003E-4</v>
+      </c>
+      <c r="J15" s="5">
+        <v>2.7E-10</v>
+      </c>
+      <c r="K15" s="2">
+        <f>STDEV(J14:J15)/SQRT(2)</f>
+        <v>2.5000000000000002E-10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -1020,34 +1029,60 @@
         <v>7</v>
       </c>
       <c r="F16" s="4">
+        <v>581000</v>
+      </c>
+      <c r="H16" s="2">
+        <v>1.01E-3</v>
+      </c>
+      <c r="J16" s="4">
+        <v>7.4300000000000002E-9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="4">
         <v>1010000</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H17" s="2">
         <v>2.1099999999999999E-3</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J17" s="4">
         <v>5.2899999999999997E-9</v>
       </c>
     </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.25">
-      <c r="F17" s="4"/>
-      <c r="H17" s="2"/>
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F18" s="4"/>
       <c r="H18" s="2"/>
       <c r="J18" s="4"/>
     </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F19" s="4"/>
       <c r="H19" s="2"/>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="F20" s="4"/>
       <c r="H20" s="2"/>
       <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="F21" s="4"/>
+      <c r="H21" s="2"/>
+      <c r="J21" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>